<commit_message>
Before changing to copy each time of template word file
</commit_message>
<xml_diff>
--- a/Book.xlsx
+++ b/Book.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Имя</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Телефон</t>
   </si>
   <si>
-    <t>Адрес</t>
-  </si>
-  <si>
     <t>Петя</t>
   </si>
   <si>
@@ -62,10 +59,19 @@
     <t>E23</t>
   </si>
   <si>
-    <t>F22</t>
-  </si>
-  <si>
-    <t>F23</t>
+    <t>адрес</t>
+  </si>
+  <si>
+    <t>Sin City</t>
+  </si>
+  <si>
+    <t>Moskvabad</t>
+  </si>
+  <si>
+    <t>Имя21</t>
+  </si>
+  <si>
+    <t>Имя22</t>
   </si>
 </sst>
 </file>
@@ -427,7 +433,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,10 +453,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -458,13 +464,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2">
         <v>902</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" s="3">
         <v>1200</v>
@@ -475,13 +481,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2">
         <v>112</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="3">
         <v>1000000000</v>
@@ -492,13 +498,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2">
         <v>222</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3">
         <v>3939</v>
@@ -576,13 +582,13 @@
       </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -590,41 +596,56 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="2">
+        <v>21</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E22" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="2">
+        <v>22</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>